<commit_message>
updating SOLD with comments from Aline on typos and fixing figures sizes
</commit_message>
<xml_diff>
--- a/Papers/An Extensible Framework to Validate and Build Dataset Profiles/figures/analysis.xlsx
+++ b/Papers/An Extensible Framework to Validate and Build Dataset Profiles/figures/analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -234,13 +234,18 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -303,13 +308,13 @@
                   <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.166666666666667</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.642857142857143</c:v>
+                  <c:v>0.6428571428571429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,10 +365,10 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -411,7 +416,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.411764705882353</c:v>
+                  <c:v>0.41176470588235292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -459,7 +464,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.166666666666667</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.8</c:v>
@@ -477,11 +482,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2051726632"/>
-        <c:axId val="-2040254648"/>
+        <c:axId val="166549760"/>
+        <c:axId val="166567936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2051726632"/>
+        <c:axId val="166549760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2040254648"/>
+        <c:crossAx val="166567936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,9 +503,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2040254648"/>
+        <c:axId val="166567936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -541,7 +547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2051726632"/>
+        <c:crossAx val="166549760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -557,7 +563,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -566,7 +572,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -632,10 +638,10 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.411764705882353</c:v>
+                  <c:v>0.41176470588235292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.166666666666667</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -683,10 +689,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -782,10 +788,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.642857142857143</c:v>
+                  <c:v>0.6428571428571429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.8</c:v>
@@ -803,11 +809,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2047349816"/>
-        <c:axId val="-2049554984"/>
+        <c:axId val="169748736"/>
+        <c:axId val="169754624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2047349816"/>
+        <c:axId val="169748736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2049554984"/>
+        <c:crossAx val="169754624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -824,9 +830,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2049554984"/>
+        <c:axId val="169754624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -854,7 +861,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2047349816"/>
+        <c:crossAx val="169748736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -870,7 +877,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -879,7 +886,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -979,7 +986,7 @@
                   <c:v>95.88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77.9</c:v>
+                  <c:v>77.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>96.91</c:v>
@@ -1018,11 +1025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2054826792"/>
-        <c:axId val="-2049129832"/>
+        <c:axId val="169783296"/>
+        <c:axId val="169785216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2054826792"/>
+        <c:axId val="169783296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1057,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2049129832"/>
+        <c:crossAx val="169785216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1058,9 +1065,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2049129832"/>
+        <c:axId val="169785216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1096,7 +1104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054826792"/>
+        <c:crossAx val="169783296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1107,7 +1115,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1116,7 +1124,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1168,22 +1176,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>212.0</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112.0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1212,7 +1220,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1668,15 +1676,15 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1690,7 +1698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1729,7 +1737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1743,7 +1751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -1758,7 +1766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1790,7 +1798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1801,7 +1809,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1814,7 +1822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1828,7 +1836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>0.6428571428571429</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1872,7 +1880,7 @@
         <v>0.41176470588235292</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1885,7 +1893,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -1899,7 +1907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -1931,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1939,7 +1947,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1955,7 +1963,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1963,7 +1971,7 @@
         <v>96.91</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1971,7 +1979,7 @@
         <v>95.88</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1979,7 +1987,7 @@
         <v>81.55</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -1987,7 +1995,7 @@
         <v>95.51</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1995,7 +2003,7 @@
         <v>6.46</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2003,7 +2011,7 @@
         <v>95.88</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2011,7 +2019,7 @@
         <v>77.900000000000006</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2019,7 +2027,7 @@
         <v>96.91</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2027,7 +2035,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -2035,7 +2043,7 @@
         <v>91.29</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2043,7 +2051,7 @@
         <v>79.87</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -2051,7 +2059,7 @@
         <v>45.69</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -2059,7 +2067,7 @@
         <v>9.18</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -2067,7 +2075,7 @@
         <v>96.82</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -2075,7 +2083,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -2083,7 +2091,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -2091,7 +2099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>33</v>
       </c>
@@ -2099,7 +2107,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2107,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -2115,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>

</xml_diff>